<commit_message>
Update Components for LCSC Availability and Complete Schematic
This commit includes the following key changes:

1. Component Replacement: All components in the design have been updated to ensure availability at LCSC. This includes substituting parts that were previously sourced from other suppliers with equivalent or better components available through LCSC. Each component has been carefully selected to maintain or enhance the performance and reliability of the design.

2. Schematic Finalization: The schematic has been thoroughly reviewed and finalized. This includes checking all connections, ensuring correct part values, and verifying that the design meets all specified requirements. The finalized schematic reflects a robust and optimized layout, ready for the next phase of PCB design.

These changes ensure smoother procurement of parts and set the stage for the upcoming PCB layout phase, aligning with project timelines and quality standards.
</commit_message>
<xml_diff>
--- a/hardware/altium/Project Outputs for AirPurity/BOM/Bill of Materials-AirPurity.xlsx
+++ b/hardware/altium/Project Outputs for AirPurity/BOM/Bill of Materials-AirPurity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\GitHub\AirPurity\hardware\altium\Project Outputs for AirPurity\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8467BC15-B335-4610-BE0D-A4E4C1FA22E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75098C82-057E-4047-A21C-8CE52BEE9791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15345" xr2:uid="{7309C59E-CDA8-408A-B67E-8C179D6FADE9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{44B75250-361C-43F6-AF40-F76D222C401F}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-AirPurity" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="163">
   <si>
     <t>Comment</t>
   </si>
@@ -95,7 +95,7 @@
     <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0201, 20pF, C0G, 30ppm/°C, 2%, 50V</t>
   </si>
   <si>
-    <t>C4, C7, C33, C34, C35, C36</t>
+    <t>C4, C7, C34, C35, C36, C37</t>
   </si>
   <si>
     <t>FP-GRM033-0_03-MFG</t>
@@ -110,7 +110,7 @@
     <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0201, 0.10uF, X5R, 15%, 10%, 10V</t>
   </si>
   <si>
-    <t>C5, C10, C15, C16, C17, C18, C21, C22, C28, C37</t>
+    <t>C5, C10, C11, C16, C17, C18, C19, C21, C28, C38, C40</t>
   </si>
   <si>
     <t>CMP-2010-01264-2</t>
@@ -128,48 +128,33 @@
     <t>CMP-06035-002174-1</t>
   </si>
   <si>
-    <t>GRM155R6YA105ME11J</t>
-  </si>
-  <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0402, 1.0uF, X5R, 15%, 20%, 35V</t>
-  </si>
-  <si>
-    <t>C11, C12, C13, C14, C19</t>
+    <t>GRM155R61H105KE05D</t>
+  </si>
+  <si>
+    <t>CERAMIC CAP, MLCC 1UF 50VDC X5R</t>
+  </si>
+  <si>
+    <t>C12, C13, C14, C15, C22, C25, C26, C27, C29, C30, C31, C32, C33, C39</t>
   </si>
   <si>
     <t>FP-GRM155-0_1-MFG</t>
   </si>
   <si>
-    <t>CMP-06035-014456-1</t>
-  </si>
-  <si>
-    <t>GRM219R61E475KA73D</t>
-  </si>
-  <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0805, 4.7uF, X5R, 15%, 10%, 25V</t>
-  </si>
-  <si>
-    <t>C23</t>
-  </si>
-  <si>
-    <t>FP-GRM219-0_15-0_1-MFG</t>
-  </si>
-  <si>
-    <t>CMP-06035-041247-1</t>
-  </si>
-  <si>
-    <t>GRM155R61H105KE05D</t>
-  </si>
-  <si>
-    <t>CERAMIC CAP, MLCC 1UF 50VDC X5R</t>
-  </si>
-  <si>
-    <t>C24, C25, C26, C27, C29, C30, C31, C32</t>
-  </si>
-  <si>
     <t>CMP-06035-026840-2</t>
   </si>
   <si>
+    <t>GRM155C61E475ME15J</t>
+  </si>
+  <si>
+    <t>Chip Multilayer Ceramic Capacitors for General Purpose 0402 Package 0.7mm 4.7uF @ 20% 25Vdc X5S @ 22%</t>
+  </si>
+  <si>
+    <t>C23, C24</t>
+  </si>
+  <si>
+    <t>CMP-06035-063317-1</t>
+  </si>
+  <si>
     <t>150060YS75000</t>
   </si>
   <si>
@@ -185,19 +170,19 @@
     <t>CMP-1426-00005-2</t>
   </si>
   <si>
-    <t>B0530WS-7-F</t>
-  </si>
-  <si>
-    <t>DIODE SCHOTTKY 30V 500MA SOD323</t>
+    <t>MBR0530</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 30V 500MA SOD123</t>
   </si>
   <si>
     <t>D2, D4, D5, D6</t>
   </si>
   <si>
-    <t>FP-SOD323-MFG</t>
-  </si>
-  <si>
-    <t>CMP-12790-000023-1</t>
+    <t>FP-425-04-MFG</t>
+  </si>
+  <si>
+    <t>CMP-2000-05113-2</t>
   </si>
   <si>
     <t>150060VS75000</t>
@@ -224,6 +209,15 @@
     <t>CMP-05590-000002-1</t>
   </si>
   <si>
+    <t>Fiducial</t>
+  </si>
+  <si>
+    <t>FD1, FD2</t>
+  </si>
+  <si>
+    <t>FIDUCIAL-1MM</t>
+  </si>
+  <si>
     <t>USB4105-GF-A</t>
   </si>
   <si>
@@ -260,7 +254,7 @@
     <t>Film type RF Inductor 3nH ±0.1nH 600mA 0.12Ω 0201 (0603)</t>
   </si>
   <si>
-    <t>L1</t>
+    <t>L1, L2</t>
   </si>
   <si>
     <t>FP-LQP03HQ_02-MFG</t>
@@ -269,34 +263,19 @@
     <t>CMP-06042-011117-1</t>
   </si>
   <si>
-    <t>LQP03TG2N0B02D</t>
-  </si>
-  <si>
-    <t>Film type RF Inductor 2nH ±0.1nH 450mA 0.25Ω 0201 (0603)</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>FP-LQP03PN_02-MFG</t>
-  </si>
-  <si>
-    <t>CMP-06042-013678-1</t>
-  </si>
-  <si>
-    <t>MLZ1608E100MT000</t>
-  </si>
-  <si>
-    <t>Shielded Multilayer Inductor 10uH ±20% 40mA 1170mΩ SMD 0603</t>
+    <t>1239AS-H-100M=P2</t>
+  </si>
+  <si>
+    <t>FIXED IND 10UH 1A 460 MOHM SMD</t>
   </si>
   <si>
     <t>L3</t>
   </si>
   <si>
-    <t>FP-MLZ1608-MFG</t>
-  </si>
-  <si>
-    <t>CMP-08253-000388-1</t>
+    <t>FP-DFE252012C-MFG</t>
+  </si>
+  <si>
+    <t>CMP-06042-012626-1</t>
   </si>
   <si>
     <t>S2B-PH-SM4-TB(LF)(SN)</t>
@@ -365,19 +344,46 @@
     <t>RES 5.1kΩ ±1% 0.063W 0402</t>
   </si>
   <si>
-    <t>R2, R3</t>
+    <t>R2, R4, R9, R10</t>
   </si>
   <si>
     <t>CMP-2002-01829-3</t>
   </si>
   <si>
+    <t>AC0402FR-0710KL</t>
+  </si>
+  <si>
+    <t>RES 10kΩ ±1% 0.063W 0402</t>
+  </si>
+  <si>
+    <t>R3, R11, R12, R14</t>
+  </si>
+  <si>
+    <t>CMP-2002-01790-3</t>
+  </si>
+  <si>
+    <t>AC0402JR-070RL</t>
+  </si>
+  <si>
+    <t>RES 0Ω 0.00% 0.063W 0402</t>
+  </si>
+  <si>
+    <t>R5, R8</t>
+  </si>
+  <si>
+    <t>FP-AC0402-IPC_A</t>
+  </si>
+  <si>
+    <t>CMP-2002-01838-3</t>
+  </si>
+  <si>
     <t>AC0402FR-07100KL</t>
   </si>
   <si>
     <t>RES 100kΩ ±1% 0.063W 0402</t>
   </si>
   <si>
-    <t>R4, R6, R11, R13, R15</t>
+    <t>R6</t>
   </si>
   <si>
     <t>FP-AC0402-IPC_B</t>
@@ -386,67 +392,31 @@
     <t>CMP-2002-01788-3</t>
   </si>
   <si>
-    <t>AC0402JR-070RL</t>
-  </si>
-  <si>
-    <t>RES 0Ω 0.00% 0.063W 0402</t>
-  </si>
-  <si>
-    <t>R5, R8</t>
-  </si>
-  <si>
-    <t>FP-AC0402-IPC_A</t>
-  </si>
-  <si>
-    <t>CMP-2002-01838-3</t>
-  </si>
-  <si>
-    <t>AC0402FR-07510KL</t>
-  </si>
-  <si>
-    <t>RES SMD 510K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>R9, R10</t>
-  </si>
-  <si>
-    <t>CMP-03412-017240-3</t>
-  </si>
-  <si>
-    <t>AC0402FR-07499RL</t>
-  </si>
-  <si>
-    <t>RES 499Ω ±1% 0.063W 0402</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>CMP-03412-031876-2</t>
-  </si>
-  <si>
     <t>AC0402FR-073RL</t>
   </si>
   <si>
     <t>RES 3Ω ±1% 0.063W 0402</t>
   </si>
   <si>
-    <t>R14</t>
+    <t>R13</t>
   </si>
   <si>
     <t>CMP-03412-050121-1</t>
   </si>
   <si>
-    <t>EVQ-P7J01P</t>
-  </si>
-  <si>
-    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
-  </si>
-  <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>FP-EVQ-P7J01P-MFG</t>
+    <t>AC0402FR-131KL</t>
+  </si>
+  <si>
+    <t>RES 1kΩ ±1% 0.063W 0402</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>FP-AC0402-IPC_C</t>
+  </si>
+  <si>
+    <t>CMP-03412-047873-1</t>
   </si>
   <si>
     <t>PTS636 SKG25 SMTR LFS</t>
@@ -455,7 +425,7 @@
     <t>TACT 6.0 X 3.5, 2.5 MM H, 250GF,</t>
   </si>
   <si>
-    <t>SW2, SW3</t>
+    <t>SW1, SW2</t>
   </si>
   <si>
     <t>FP-PTS636_SKG25_SMTR_LFS-MFG</t>
@@ -503,13 +473,28 @@
     <t>PSON80P300X300X100-8N</t>
   </si>
   <si>
+    <t>MAX17043X+T10</t>
+  </si>
+  <si>
+    <t>IC FUEL GAUGE LI-ION 1CELL 9UCSP</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>FP-W91C1-1-MFG</t>
+  </si>
+  <si>
+    <t>CMP-05715-000141-1</t>
+  </si>
+  <si>
     <t>ESP32-C3FH4</t>
   </si>
   <si>
     <t>Bluetooth, WiFi 802.11b/g/n, Bluetooth v5.0 Transceiver Module 2.402GHz ~ 2.48GHz Antenna Not Included Surface Mount</t>
   </si>
   <si>
-    <t>U4</t>
+    <t>U5</t>
   </si>
   <si>
     <t>QFN50P500X500X90-33N</t>
@@ -938,14 +923,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FE39BE-8B12-46F5-8DBF-229E90300212}">
-  <dimension ref="A1:F36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D61ACE-E294-4267-A4E3-0DE6F0CC28FD}">
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1045,7 +1037,7 @@
         <v>24</v>
       </c>
       <c r="F5" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1085,7 +1077,7 @@
         <v>33</v>
       </c>
       <c r="F7" s="1">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1099,33 +1091,33 @@
         <v>36</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1145,7 +1137,7 @@
         <v>47</v>
       </c>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1153,33 +1145,33 @@
         <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="F11" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>55</v>
@@ -1193,36 +1185,36 @@
         <v>56</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -1230,19 +1222,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
@@ -1250,39 +1242,39 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="F16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -1290,19 +1282,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
@@ -1310,19 +1302,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -1330,19 +1322,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
@@ -1350,139 +1342,139 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="F21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="F22" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="F23" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="F24" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="F25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="F26" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
@@ -1490,39 +1482,39 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="F28" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
@@ -1539,30 +1531,30 @@
         <v>138</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="F30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="E31" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
@@ -1570,19 +1562,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
@@ -1590,19 +1582,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
@@ -1610,19 +1602,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
@@ -1645,26 +1637,6 @@
         <v>162</v>
       </c>
       <c r="F35" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F36" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refinement of Schematic and Component Adjustments
This commit introduces a set of minor yet significant refinements:

1. Schematic Tweaks: Minor adjustments have been made to the schematic for enhanced clarity and functionality. These include optimizing trace routes, revising component labels for better readability, and minor corrections to ensure alignment with design standards.

2. Component Updates: A few components have been replaced or adjusted to better suit the design requirements and to ensure greater availability. This includes selecting alternative parts from LCSC that are more cost-effective or offer better performance.

These small changes are part of our ongoing effort to optimize the design for manufacturability and efficiency. The adjustments are critical to maintaining the integrity and performance of the final product while ensuring a smooth transition to the PCB layout phase.
</commit_message>
<xml_diff>
--- a/hardware/altium/Project Outputs for AirPurity/BOM/Bill of Materials-AirPurity.xlsx
+++ b/hardware/altium/Project Outputs for AirPurity/BOM/Bill of Materials-AirPurity.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\GitHub\AirPurity\hardware\altium\Project Outputs for AirPurity\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75098C82-057E-4047-A21C-8CE52BEE9791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{72D11000-BE15-4B8A-B7F0-B3DFD548A258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{44B75250-361C-43F6-AF40-F76D222C401F}"/>
+    <workbookView xWindow="7770" yWindow="345" windowWidth="28800" windowHeight="15345" xr2:uid="{0DA47330-5165-4C07-B1BD-391E85D90674}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-AirPurity" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="151">
   <si>
     <t>Comment</t>
   </si>
@@ -59,7 +59,7 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>ANT3216A063R2400A</t>
+    <t>ANT016008LCS2442MA2</t>
   </si>
   <si>
     <t>RF ANT 2.4GHZ CHIP SOLDER SMD</t>
@@ -68,94 +68,85 @@
     <t>ANT1</t>
   </si>
   <si>
-    <t>FP-ANT3216A063R2400A-MFG</t>
-  </si>
-  <si>
-    <t>CMP-16379-000004-1</t>
-  </si>
-  <si>
-    <t>GRM155R61A106ME11D</t>
-  </si>
-  <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0402, 10uF, X5R, 15%, 20%, 10V</t>
-  </si>
-  <si>
-    <t>C1, C2, C3, C6, C20</t>
+    <t>FP-ANT016008LCS2442MA2-0</t>
+  </si>
+  <si>
+    <t>CMP-08339-000002-1</t>
+  </si>
+  <si>
+    <t>GRM155R61E475ME15D</t>
+  </si>
+  <si>
+    <t>Chip Multilayer Ceramic Capacitors for General Purpose 0402 Package 0.7mm 4.7uF @ 20% 25Vdc X5S @ 22%</t>
+  </si>
+  <si>
+    <t>C1, C3, C22, C27</t>
   </si>
   <si>
     <t>FP-GRM155-0_2-MFG</t>
   </si>
   <si>
-    <t>CMP-06035-026070-1</t>
-  </si>
-  <si>
-    <t>GRM0335C1H200GA01D</t>
-  </si>
-  <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0201, 20pF, C0G, 30ppm/°C, 2%, 50V</t>
-  </si>
-  <si>
-    <t>C4, C7, C34, C35, C36, C37</t>
+    <t>CMP-06035-063317-1</t>
+  </si>
+  <si>
+    <t>GRM155R61E105KA12D</t>
+  </si>
+  <si>
+    <t>CERAMIC CAP, MLCC 1UF 50VDC X5R</t>
+  </si>
+  <si>
+    <t>C2, C6, C10, C11, C12, C13, C14, C19, C21, C23, C24, C25, C28, C29, C30, C31, C32</t>
+  </si>
+  <si>
+    <t>FP-GRM155-0_1-MFG</t>
+  </si>
+  <si>
+    <t>CMP-06035-026840-2</t>
+  </si>
+  <si>
+    <t>GRM033R61A104KE15D</t>
+  </si>
+  <si>
+    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0201, 0.10uF, X5R, 15%, 10%, 10V</t>
+  </si>
+  <si>
+    <t>C4, C5, C7, C8, C9, C15, C16, C17, C18, C20, C26, C37</t>
   </si>
   <si>
     <t>FP-GRM033-0_03-MFG</t>
   </si>
   <si>
-    <t>CMP-2010-01522-2</t>
-  </si>
-  <si>
-    <t>GRM033R61A104KE15D</t>
-  </si>
-  <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0201, 0.10uF, X5R, 15%, 10%, 10V</t>
-  </si>
-  <si>
-    <t>C5, C10, C11, C16, C17, C18, C19, C21, C28, C38, C40</t>
-  </si>
-  <si>
     <t>CMP-2010-01264-2</t>
   </si>
   <si>
-    <t>GRM0335C1H1R5BA01J</t>
-  </si>
-  <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0201, 1.5pF, C0G, 30ppm/°C, 0.1pF, 50V</t>
-  </si>
-  <si>
-    <t>C8, C9</t>
-  </si>
-  <si>
-    <t>CMP-06035-002174-1</t>
-  </si>
-  <si>
-    <t>GRM155R61H105KE05D</t>
-  </si>
-  <si>
-    <t>CERAMIC CAP, MLCC 1UF 50VDC X5R</t>
-  </si>
-  <si>
-    <t>C12, C13, C14, C15, C22, C25, C26, C27, C29, C30, C31, C32, C33, C39</t>
-  </si>
-  <si>
-    <t>FP-GRM155-0_1-MFG</t>
-  </si>
-  <si>
-    <t>CMP-06035-026840-2</t>
-  </si>
-  <si>
-    <t>GRM155C61E475ME15J</t>
-  </si>
-  <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose 0402 Package 0.7mm 4.7uF @ 20% 25Vdc X5S @ 22%</t>
-  </si>
-  <si>
-    <t>C23, C24</t>
-  </si>
-  <si>
-    <t>CMP-06035-063317-1</t>
-  </si>
-  <si>
-    <t>150060YS75000</t>
+    <t>GRM0335C1H150FA01D</t>
+  </si>
+  <si>
+    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0201, 15pF, C0G, 30ppm/°C, 1%, 50V</t>
+  </si>
+  <si>
+    <t>C33, C34</t>
+  </si>
+  <si>
+    <t>FP-GRM033-0_03-IPC_B</t>
+  </si>
+  <si>
+    <t>CMP-06035-001503-1</t>
+  </si>
+  <si>
+    <t>GRM0335C1H180FA01D</t>
+  </si>
+  <si>
+    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0201, 18pF, C0G, 30ppm/°C, 1%, 50V</t>
+  </si>
+  <si>
+    <t>C35, C36</t>
+  </si>
+  <si>
+    <t>CMP-06035-028008-1</t>
+  </si>
+  <si>
+    <t>150060BS75000</t>
   </si>
   <si>
     <t/>
@@ -167,10 +158,10 @@
     <t>WL-SMCW_0603_150060xx75000</t>
   </si>
   <si>
-    <t>CMP-1426-00005-2</t>
-  </si>
-  <si>
-    <t>MBR0530</t>
+    <t>CMP-1426-00003-3</t>
+  </si>
+  <si>
+    <t>MBR0530T3G</t>
   </si>
   <si>
     <t>DIODE SCHOTTKY 30V 500MA SOD123</t>
@@ -185,28 +176,28 @@
     <t>CMP-2000-05113-2</t>
   </si>
   <si>
-    <t>150060VS75000</t>
+    <t>150060GS75000</t>
   </si>
   <si>
     <t>D3</t>
   </si>
   <si>
-    <t>CMP-1426-00006-6</t>
-  </si>
-  <si>
-    <t>ERB-RD0R50X</t>
-  </si>
-  <si>
-    <t>FUSE BOARD MNT 500MA 32VDC 0402</t>
+    <t>CMP-1426-00002-3</t>
+  </si>
+  <si>
+    <t>0466.500NRHF</t>
+  </si>
+  <si>
+    <t>FUSE BOARD MOUNT 500MA 63VAC/VDC</t>
   </si>
   <si>
     <t>F1</t>
   </si>
   <si>
-    <t>FP-ERBRD-MFG</t>
-  </si>
-  <si>
-    <t>CMP-05590-000002-1</t>
+    <t>FP-0466-MFG</t>
+  </si>
+  <si>
+    <t>CMP-08605-000090-1</t>
   </si>
   <si>
     <t>Fiducial</t>
@@ -218,7 +209,7 @@
     <t>FIDUCIAL-1MM</t>
   </si>
   <si>
-    <t>USB4105-GF-A</t>
+    <t>CX90M-16P</t>
   </si>
   <si>
     <t>CONN RCPT USB2.0 TYPEC 5A</t>
@@ -233,7 +224,7 @@
     <t>CMP-245163-000001-1</t>
   </si>
   <si>
-    <t>505110-2491</t>
+    <t>524352471</t>
   </si>
   <si>
     <t>CONN FFC/FPC BOTTOM 24P .5MM R/A</t>
@@ -248,19 +239,19 @@
     <t>CMP-04775-000015-1</t>
   </si>
   <si>
-    <t>LQP03HQ3N0B02D</t>
-  </si>
-  <si>
-    <t>Film type RF Inductor 3nH ±0.1nH 600mA 0.12Ω 0201 (0603)</t>
-  </si>
-  <si>
-    <t>L1, L2</t>
-  </si>
-  <si>
-    <t>FP-LQP03HQ_02-MFG</t>
-  </si>
-  <si>
-    <t>CMP-06042-011117-1</t>
+    <t>LQP03TN2N1BZ2D</t>
+  </si>
+  <si>
+    <t>Film type RF Inductor for Automotive 2.1nH ±0.1nH 600mA 0.15Ω 0201 (0603)</t>
+  </si>
+  <si>
+    <t>L1, L2, L3</t>
+  </si>
+  <si>
+    <t>FP-LQP03TG_02-IPC_B</t>
+  </si>
+  <si>
+    <t>CMP-06042-011982-1</t>
   </si>
   <si>
     <t>1239AS-H-100M=P2</t>
@@ -269,7 +260,7 @@
     <t>FIXED IND 10UH 1A 460 MOHM SMD</t>
   </si>
   <si>
-    <t>L3</t>
+    <t>L4</t>
   </si>
   <si>
     <t>FP-DFE252012C-MFG</t>
@@ -293,37 +284,37 @@
     <t>CMP-1755-00001-1</t>
   </si>
   <si>
-    <t>BSS84LT1G</t>
-  </si>
-  <si>
-    <t>MOSFET P-CH 50V 130MA SOT-23</t>
+    <t>DMP2165UW-7</t>
+  </si>
+  <si>
+    <t>MOSFET BVDSS: 8V-24V SOT323 T&amp;R</t>
   </si>
   <si>
     <t>Q1</t>
   </si>
   <si>
-    <t>FP-318-08-MFG</t>
-  </si>
-  <si>
-    <t>CMP-1058-00762-2</t>
-  </si>
-  <si>
-    <t>SI1308EDL-T1-BE3</t>
-  </si>
-  <si>
-    <t>SI1308EDL-T1-BE3 Single N-Channel 30 V 0.4 W 4.1 nC Silicon Surface Mount - SOT-323</t>
+    <t>FP-SOT323-IPC_B</t>
+  </si>
+  <si>
+    <t>CMP-12801-000112-1</t>
+  </si>
+  <si>
+    <t>SI1308EDL-T1-GE3</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 30V 1.4A SC-70-3</t>
   </si>
   <si>
     <t>Q2</t>
   </si>
   <si>
-    <t>FP-S-03946-MFG</t>
-  </si>
-  <si>
-    <t>CMP-00030-113152034-1</t>
-  </si>
-  <si>
-    <t>AC0402FR-07150RL</t>
+    <t>FP-5549-MFG</t>
+  </si>
+  <si>
+    <t>CMP-02550-000099-2</t>
+  </si>
+  <si>
+    <t>RC0402FR-07150RL</t>
   </si>
   <si>
     <t>RES 150Ω ±1% 0.063W 0402</t>
@@ -338,7 +329,7 @@
     <t>CMP-2002-01794-3</t>
   </si>
   <si>
-    <t>AC0402FR-075K1L</t>
+    <t>RC0402FR-075K1L</t>
   </si>
   <si>
     <t>RES 5.1kΩ ±1% 0.063W 0402</t>
@@ -350,19 +341,19 @@
     <t>CMP-2002-01829-3</t>
   </si>
   <si>
-    <t>AC0402FR-0710KL</t>
+    <t>RC0402FR-0710KL</t>
   </si>
   <si>
     <t>RES 10kΩ ±1% 0.063W 0402</t>
   </si>
   <si>
-    <t>R3, R11, R12, R14</t>
+    <t>R3, R6, R11, R12, R14</t>
   </si>
   <si>
     <t>CMP-2002-01790-3</t>
   </si>
   <si>
-    <t>AC0402JR-070RL</t>
+    <t>RC0402FR-0722RL</t>
   </si>
   <si>
     <t>RES 0Ω 0.00% 0.063W 0402</t>
@@ -377,22 +368,7 @@
     <t>CMP-2002-01838-3</t>
   </si>
   <si>
-    <t>AC0402FR-07100KL</t>
-  </si>
-  <si>
-    <t>RES 100kΩ ±1% 0.063W 0402</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>FP-AC0402-IPC_B</t>
-  </si>
-  <si>
-    <t>CMP-2002-01788-3</t>
-  </si>
-  <si>
-    <t>AC0402FR-073RL</t>
+    <t>RC0402FR-072R37L</t>
   </si>
   <si>
     <t>RES 3Ω ±1% 0.063W 0402</t>
@@ -404,22 +380,7 @@
     <t>CMP-03412-050121-1</t>
   </si>
   <si>
-    <t>AC0402FR-131KL</t>
-  </si>
-  <si>
-    <t>RES 1kΩ ±1% 0.063W 0402</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>FP-AC0402-IPC_C</t>
-  </si>
-  <si>
-    <t>CMP-03412-047873-1</t>
-  </si>
-  <si>
-    <t>PTS636 SKG25 SMTR LFS</t>
+    <t>PTS636 SK25J SMTR LFS</t>
   </si>
   <si>
     <t>TACT 6.0 X 3.5, 2.5 MM H, 250GF,</t>
@@ -449,16 +410,34 @@
     <t>CMP-0133-00143-2</t>
   </si>
   <si>
-    <t>MIC5504-3.3YM5-TR</t>
-  </si>
-  <si>
-    <t>IC REG LINEAR 3.3V 300MA SOT23-5</t>
+    <t>TLV70233DBVR</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
   <si>
     <t>U2</t>
   </si>
   <si>
-    <t>CMP-2000-07604-2</t>
+    <t>FP-DBV0005A-MFG</t>
+  </si>
+  <si>
+    <t>CMP-0394-00528-4</t>
+  </si>
+  <si>
+    <t>MAX17048G+T10</t>
+  </si>
+  <si>
+    <t>IC FUEL GAUGE LI-ION 1CELL 8WLP</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>FP-W80B1-1-MFG</t>
+  </si>
+  <si>
+    <t>CMP-05715-000033-1</t>
   </si>
   <si>
     <t>BME680</t>
@@ -467,27 +446,12 @@
     <t>Gas, Humidity, Pressure, Temperature Sensor IÂ²C, SPI Output</t>
   </si>
   <si>
-    <t>U3</t>
+    <t>U4</t>
   </si>
   <si>
     <t>PSON80P300X300X100-8N</t>
   </si>
   <si>
-    <t>MAX17043X+T10</t>
-  </si>
-  <si>
-    <t>IC FUEL GAUGE LI-ION 1CELL 9UCSP</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>FP-W91C1-1-MFG</t>
-  </si>
-  <si>
-    <t>CMP-05715-000141-1</t>
-  </si>
-  <si>
     <t>ESP32-C3FH4</t>
   </si>
   <si>
@@ -500,7 +464,7 @@
     <t>QFN50P500X500X90-33N</t>
   </si>
   <si>
-    <t>ABS07AIG-32.768KHZ-7-D-T</t>
+    <t>9H03200031</t>
   </si>
   <si>
     <t>Crystal 32.768kHz ±20ppm (Tol) 7pF FUND 70kΩ Automotive 2-Pin Mini-CSMD T/R</t>
@@ -515,7 +479,7 @@
     <t>CMP-27762-015608-1</t>
   </si>
   <si>
-    <t>ABM11-40.000MHZ-B1U-T3</t>
+    <t>7M40000183</t>
   </si>
   <si>
     <t>Crystal 40MHz ±10ppm 10pF SMD-4 2mm x 1.6mm</t>
@@ -538,7 +502,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -618,39 +582,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -702,7 +666,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -813,6 +777,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -821,13 +792,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -892,52 +856,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D61ACE-E294-4267-A4E3-0DE6F0CC28FD}">
-  <dimension ref="A1:F35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0053D76D-044A-41D0-9605-62B39F81CC81}">
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="109.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="1" max="6" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -997,7 +934,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1017,7 +954,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="1">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1031,30 +968,30 @@
         <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
@@ -1062,82 +999,82 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="1">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F9" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F10" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1145,16 +1082,16 @@
         <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
@@ -1162,22 +1099,22 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1185,36 +1122,36 @@
         <v>56</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -1222,59 +1159,59 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F15" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -1282,19 +1219,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
@@ -1302,19 +1239,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -1322,139 +1259,139 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F21" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F22" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F23" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F25" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
@@ -1462,19 +1399,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
@@ -1482,39 +1419,39 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
@@ -1522,19 +1459,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
@@ -1542,19 +1479,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
@@ -1562,81 +1499,21 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F33" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F35" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initiation of Custom Integrated Library Development
In this commit, we embark on the development of a custom integrated library for our project. Key highlights include:

1. Foundation Setup: Established the basic structure of the integrated library. This includes setting up directories, initializing standard file formats, and defining the initial set of components to be included in the library.

2. Component Inclusion: Began populating the library with essential components. Initial focus is on the components that are unique to our project or those that are frequently used. Each component entry includes its schematic symbol, PCB footprint, and any necessary 3D models.
</commit_message>
<xml_diff>
--- a/hardware/altium/Project Outputs for AirPurity/BOM/Bill of Materials-AirPurity.xlsx
+++ b/hardware/altium/Project Outputs for AirPurity/BOM/Bill of Materials-AirPurity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\GitHub\AirPurity\hardware\altium\Project Outputs for AirPurity\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72D11000-BE15-4B8A-B7F0-B3DFD548A258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CCEBFFF-5ADA-41CC-9F5B-081745CA855F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7770" yWindow="345" windowWidth="28800" windowHeight="15345" xr2:uid="{0DA47330-5165-4C07-B1BD-391E85D90674}"/>
+    <workbookView xWindow="7770" yWindow="345" windowWidth="28800" windowHeight="15345" xr2:uid="{F0698127-BF11-446B-A619-86CDEC576054}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-AirPurity" sheetId="1" r:id="rId1"/>
@@ -867,7 +867,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0053D76D-044A-41D0-9605-62B39F81CC81}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6A5DBB-F705-4291-A87E-D24BE04BD405}">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Update Rules and Template and Library
Updated Rules Templates and Library
</commit_message>
<xml_diff>
--- a/hardware/altium/Project Outputs for AirPurity/BOM/Bill of Materials-AirPurity.xlsx
+++ b/hardware/altium/Project Outputs for AirPurity/BOM/Bill of Materials-AirPurity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\GitHub\AirPurity\hardware\altium\Project Outputs for AirPurity\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CCEBFFF-5ADA-41CC-9F5B-081745CA855F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAF1172D-4F73-4018-A035-F023C5D25364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7770" yWindow="345" windowWidth="28800" windowHeight="15345" xr2:uid="{F0698127-BF11-446B-A619-86CDEC576054}"/>
+    <workbookView xWindow="1260" yWindow="0" windowWidth="28800" windowHeight="15345" xr2:uid="{D14EC731-8949-4434-9712-2FC18A352472}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-AirPurity" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="128">
   <si>
     <t>Comment</t>
   </si>
@@ -50,406 +50,343 @@
     <t>Designator</t>
   </si>
   <si>
-    <t>Footprint</t>
-  </si>
-  <si>
     <t>LibRef</t>
   </si>
   <si>
+    <t>LCSC Part Number</t>
+  </si>
+  <si>
     <t>Quantity</t>
   </si>
   <si>
     <t>ANT016008LCS2442MA2</t>
   </si>
   <si>
-    <t>RF ANT 2.4GHZ CHIP SOLDER SMD</t>
+    <t>RF ANT 2.4GHZ</t>
   </si>
   <si>
     <t>ANT1</t>
   </si>
   <si>
-    <t>FP-ANT016008LCS2442MA2-0</t>
-  </si>
-  <si>
-    <t>CMP-08339-000002-1</t>
+    <t>C209892</t>
+  </si>
+  <si>
+    <t>GRM155R61E105KA12D</t>
+  </si>
+  <si>
+    <t>1uF X5R 0402 Multilayer Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>C1, C6, C10, C11, C12, C13, C14, C19, C20, C22, C23, C24, C25, C27, C29, C30, C32</t>
+  </si>
+  <si>
+    <t>C77009</t>
   </si>
   <si>
     <t>GRM155R61E475ME15D</t>
   </si>
   <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose 0402 Package 0.7mm 4.7uF @ 20% 25Vdc X5S @ 22%</t>
-  </si>
-  <si>
-    <t>C1, C3, C22, C27</t>
-  </si>
-  <si>
-    <t>FP-GRM155-0_2-MFG</t>
-  </si>
-  <si>
-    <t>CMP-06035-063317-1</t>
-  </si>
-  <si>
-    <t>GRM155R61E105KA12D</t>
-  </si>
-  <si>
-    <t>CERAMIC CAP, MLCC 1UF 50VDC X5R</t>
-  </si>
-  <si>
-    <t>C2, C6, C10, C11, C12, C13, C14, C19, C21, C23, C24, C25, C28, C29, C30, C31, C32</t>
-  </si>
-  <si>
-    <t>FP-GRM155-0_1-MFG</t>
-  </si>
-  <si>
-    <t>CMP-06035-026840-2</t>
+    <t>4.7uF X5R 0402 Multilayer Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>C2, C3, C26, C31</t>
+  </si>
+  <si>
+    <t>C2858031</t>
   </si>
   <si>
     <t>GRM033R61A104KE15D</t>
   </si>
   <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0201, 0.10uF, X5R, 15%, 10%, 10V</t>
-  </si>
-  <si>
-    <t>C4, C5, C7, C8, C9, C15, C16, C17, C18, C20, C26, C37</t>
-  </si>
-  <si>
-    <t>FP-GRM033-0_03-MFG</t>
-  </si>
-  <si>
-    <t>CMP-2010-01264-2</t>
+    <t>100nF X5R 0201 Multilayer Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>C4, C8, C9, C15, C16, C17, C18, C21, C28, C37</t>
+  </si>
+  <si>
+    <t>C76934</t>
   </si>
   <si>
     <t>GRM0335C1H150FA01D</t>
   </si>
   <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0201, 15pF, C0G, 30ppm/°C, 1%, 50V</t>
-  </si>
-  <si>
-    <t>C33, C34</t>
-  </si>
-  <si>
-    <t>FP-GRM033-0_03-IPC_B</t>
-  </si>
-  <si>
-    <t>CMP-06035-001503-1</t>
+    <t>15pF C0G 0201 Multilayer Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>C5, C7, C33, C34</t>
+  </si>
+  <si>
+    <t>C237567</t>
   </si>
   <si>
     <t>GRM0335C1H180FA01D</t>
   </si>
   <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0201, 18pF, C0G, 30ppm/°C, 1%, 50V</t>
+    <t>18pF C0G 0201 Multilayer Ceramic Capacitor</t>
   </si>
   <si>
     <t>C35, C36</t>
   </si>
   <si>
-    <t>CMP-06035-028008-1</t>
+    <t>C384967</t>
+  </si>
+  <si>
+    <t>MBR0530T3G</t>
+  </si>
+  <si>
+    <t>Schottky Barrier Diodes</t>
+  </si>
+  <si>
+    <t>D1, D4, D5, D6</t>
+  </si>
+  <si>
+    <t>C236079</t>
   </si>
   <si>
     <t>150060BS75000</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>WL-SMCW_0603_150060xx75000</t>
-  </si>
-  <si>
-    <t>CMP-1426-00003-3</t>
-  </si>
-  <si>
-    <t>MBR0530T3G</t>
-  </si>
-  <si>
-    <t>DIODE SCHOTTKY 30V 500MA SOD123</t>
-  </si>
-  <si>
-    <t>D2, D4, D5, D6</t>
-  </si>
-  <si>
-    <t>FP-425-04-MFG</t>
-  </si>
-  <si>
-    <t>CMP-2000-05113-2</t>
+    <t>LED Blue 3.2V 0603</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>C5197644</t>
   </si>
   <si>
     <t>150060GS75000</t>
   </si>
   <si>
+    <t>LED Emerald 3.2V 0603</t>
+  </si>
+  <si>
     <t>D3</t>
   </si>
   <si>
-    <t>CMP-1426-00002-3</t>
+    <t>C5252984</t>
   </si>
   <si>
     <t>0466.500NRHF</t>
   </si>
   <si>
-    <t>FUSE BOARD MOUNT 500MA 63VAC/VDC</t>
+    <t>Fuse 500mA</t>
   </si>
   <si>
     <t>F1</t>
   </si>
   <si>
-    <t>FP-0466-MFG</t>
-  </si>
-  <si>
-    <t>CMP-08605-000090-1</t>
+    <t>C151133</t>
   </si>
   <si>
     <t>Fiducial</t>
   </si>
   <si>
-    <t>FD1, FD2</t>
-  </si>
-  <si>
-    <t>FIDUCIAL-1MM</t>
+    <t>FD1, FD2, FD3, FD4</t>
   </si>
   <si>
     <t>CX90M-16P</t>
   </si>
   <si>
-    <t>CONN RCPT USB2.0 TYPEC 5A</t>
+    <t>Connector USB2.0 TYPE-C 16POS</t>
   </si>
   <si>
     <t>J1</t>
   </si>
   <si>
-    <t>FP-USB4105-GF-A-MFG</t>
-  </si>
-  <si>
-    <t>CMP-245163-000001-1</t>
+    <t>C2889324</t>
   </si>
   <si>
     <t>524352471</t>
   </si>
   <si>
-    <t>CONN FFC/FPC BOTTOM 24P .5MM R/A</t>
+    <t>FPC Connector, 2.0 mm, 0.5 mm, Right Angle</t>
   </si>
   <si>
     <t>J2</t>
   </si>
   <si>
-    <t>FP-505110-2491-MFG</t>
-  </si>
-  <si>
-    <t>CMP-04775-000015-1</t>
+    <t>C122394</t>
   </si>
   <si>
     <t>LQP03TN2N1BZ2D</t>
   </si>
   <si>
-    <t>Film type RF Inductor for Automotive 2.1nH ±0.1nH 600mA 0.15Ω 0201 (0603)</t>
+    <t>Inductor 2.1nH</t>
   </si>
   <si>
     <t>L1, L2, L3</t>
   </si>
   <si>
-    <t>FP-LQP03TG_02-IPC_B</t>
-  </si>
-  <si>
-    <t>CMP-06042-011982-1</t>
+    <t>C560038</t>
   </si>
   <si>
     <t>1239AS-H-100M=P2</t>
   </si>
   <si>
-    <t>FIXED IND 10UH 1A 460 MOHM SMD</t>
+    <t>Inductor 10uH</t>
   </si>
   <si>
     <t>L4</t>
   </si>
   <si>
-    <t>FP-DFE252012C-MFG</t>
-  </si>
-  <si>
-    <t>CMP-06042-012626-1</t>
+    <t>C237599</t>
   </si>
   <si>
     <t>S2B-PH-SM4-TB(LF)(SN)</t>
   </si>
   <si>
-    <t>Male Header, Pitch 2 mm, 1 x 2 Position, Height 5.5 mm, -25 to 85 degC, RoHS, Tape and Reel</t>
+    <t>Male Header, Pitch 2 mm, 1 x 2 Position</t>
   </si>
   <si>
     <t>P1</t>
   </si>
   <si>
-    <t>JST- S2B-PH-SM4-TB(LF)(SN)-2_V</t>
-  </si>
-  <si>
-    <t>CMP-1755-00001-1</t>
+    <t>C295747</t>
   </si>
   <si>
     <t>DMP2165UW-7</t>
   </si>
   <si>
-    <t>MOSFET BVDSS: 8V-24V SOT323 T&amp;R</t>
+    <t>MOSFET P-Channel</t>
   </si>
   <si>
     <t>Q1</t>
   </si>
   <si>
-    <t>FP-SOT323-IPC_B</t>
-  </si>
-  <si>
-    <t>CMP-12801-000112-1</t>
+    <t>C388477</t>
   </si>
   <si>
     <t>SI1308EDL-T1-GE3</t>
   </si>
   <si>
-    <t>MOSFET N-CH 30V 1.4A SC-70-3</t>
+    <t>MOSFET N-Channel</t>
   </si>
   <si>
     <t>Q2</t>
   </si>
   <si>
-    <t>FP-5549-MFG</t>
-  </si>
-  <si>
-    <t>CMP-02550-000099-2</t>
+    <t>C469327</t>
+  </si>
+  <si>
+    <t>RC0402FR-075K1L</t>
+  </si>
+  <si>
+    <t>5.1kΩ 0402 Chip Resistor</t>
+  </si>
+  <si>
+    <t>R1, R3, R9, R10</t>
+  </si>
+  <si>
+    <t>C105872</t>
   </si>
   <si>
     <t>RC0402FR-07150RL</t>
   </si>
   <si>
-    <t>RES 150Ω ±1% 0.063W 0402</t>
-  </si>
-  <si>
-    <t>R1, R7</t>
-  </si>
-  <si>
-    <t>FP-AC0402-MFG</t>
-  </si>
-  <si>
-    <t>CMP-2002-01794-3</t>
-  </si>
-  <si>
-    <t>RC0402FR-075K1L</t>
-  </si>
-  <si>
-    <t>RES 5.1kΩ ±1% 0.063W 0402</t>
-  </si>
-  <si>
-    <t>R2, R4, R9, R10</t>
-  </si>
-  <si>
-    <t>CMP-2002-01829-3</t>
+    <t>150Ω 0402 Chip Resistor</t>
+  </si>
+  <si>
+    <t>R2, R7</t>
+  </si>
+  <si>
+    <t>C138054</t>
   </si>
   <si>
     <t>RC0402FR-0710KL</t>
   </si>
   <si>
-    <t>RES 10kΩ ±1% 0.063W 0402</t>
-  </si>
-  <si>
-    <t>R3, R6, R11, R12, R14</t>
-  </si>
-  <si>
-    <t>CMP-2002-01790-3</t>
+    <t>10kΩ 0402 Chip Resistor</t>
+  </si>
+  <si>
+    <t>R4, R5, R11, R12, R14</t>
+  </si>
+  <si>
+    <t>C60490</t>
   </si>
   <si>
     <t>RC0402FR-0722RL</t>
   </si>
   <si>
-    <t>RES 0Ω 0.00% 0.063W 0402</t>
-  </si>
-  <si>
-    <t>R5, R8</t>
-  </si>
-  <si>
-    <t>FP-AC0402-IPC_A</t>
-  </si>
-  <si>
-    <t>CMP-2002-01838-3</t>
+    <t>22Ω 0402 Chip Resistor</t>
+  </si>
+  <si>
+    <t>R6, R8</t>
+  </si>
+  <si>
+    <t>C114765</t>
   </si>
   <si>
     <t>RC0402FR-072R37L</t>
   </si>
   <si>
-    <t>RES 3Ω ±1% 0.063W 0402</t>
+    <t>2.37Ω 0402 Chip Resistor</t>
   </si>
   <si>
     <t>R13</t>
   </si>
   <si>
-    <t>CMP-03412-050121-1</t>
+    <t>C477648</t>
   </si>
   <si>
     <t>PTS636 SK25J SMTR LFS</t>
   </si>
   <si>
-    <t>TACT 6.0 X 3.5, 2.5 MM H, 250GF,</t>
+    <t>Tactile Switch SPST</t>
   </si>
   <si>
     <t>SW1, SW2</t>
   </si>
   <si>
-    <t>FP-PTS636_SKG25_SMTR_LFS-MFG</t>
-  </si>
-  <si>
-    <t>CMP-10040-000025-1</t>
+    <t>C2800965</t>
+  </si>
+  <si>
+    <t>TLV70233DBVR</t>
+  </si>
+  <si>
+    <t>LDO Voltage Regulators 300mALow IQLDO Reg</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>C26833</t>
   </si>
   <si>
     <t>MCP73831T-2ACI/OT</t>
   </si>
   <si>
-    <t>IC CONTROLLR LI-ION 4.2V SOT23-5</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>FP-SOT23-5LD-PL-1-MFG</t>
-  </si>
-  <si>
-    <t>CMP-0133-00143-2</t>
-  </si>
-  <si>
-    <t>TLV70233DBVR</t>
-  </si>
-  <si>
-    <t>None</t>
+    <t>IC Controller LI-ION 4.2V</t>
   </si>
   <si>
     <t>U2</t>
   </si>
   <si>
-    <t>FP-DBV0005A-MFG</t>
-  </si>
-  <si>
-    <t>CMP-0394-00528-4</t>
+    <t>C424093</t>
   </si>
   <si>
     <t>MAX17048G+T10</t>
   </si>
   <si>
-    <t>IC FUEL GAUGE LI-ION 1CELL 8WLP</t>
+    <t>Fuel Gauge LI-ION</t>
   </si>
   <si>
     <t>U3</t>
   </si>
   <si>
-    <t>FP-W80B1-1-MFG</t>
-  </si>
-  <si>
-    <t>CMP-05715-000033-1</t>
+    <t>C2682616</t>
   </si>
   <si>
     <t>BME680</t>
   </si>
   <si>
-    <t>Gas, Humidity, Pressure, Temperature Sensor IÂ²C, SPI Output</t>
+    <t>Gas, Humidity, Pressure, Temperature Sensor I²C</t>
   </si>
   <si>
     <t>U4</t>
   </si>
   <si>
-    <t>PSON80P300X300X100-8N</t>
+    <t>C125972</t>
   </si>
   <si>
     <t>ESP32-C3FH4</t>
@@ -461,37 +398,31 @@
     <t>U5</t>
   </si>
   <si>
-    <t>QFN50P500X500X90-33N</t>
+    <t>C2858491</t>
   </si>
   <si>
     <t>9H03200031</t>
   </si>
   <si>
-    <t>Crystal 32.768kHz ±20ppm (Tol) 7pF FUND 70kΩ Automotive 2-Pin Mini-CSMD T/R</t>
+    <t>Crystal 32.768 kHz</t>
   </si>
   <si>
     <t>Y1</t>
   </si>
   <si>
-    <t>FP-ABS07AIG-MFG</t>
-  </si>
-  <si>
-    <t>CMP-27762-015608-1</t>
+    <t>C90944</t>
   </si>
   <si>
     <t>7M40000183</t>
   </si>
   <si>
-    <t>Crystal 40MHz ±10ppm 10pF SMD-4 2mm x 1.6mm</t>
+    <t>Crystal 40 MHz</t>
   </si>
   <si>
     <t>Y2</t>
   </si>
   <si>
-    <t>FP-ABM11-MFG</t>
-  </si>
-  <si>
-    <t>CMP-27762-013416-1</t>
+    <t>C331598</t>
   </si>
 </sst>
 </file>
@@ -867,14 +798,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6A5DBB-F705-4291-A87E-D24BE04BD405}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5E92E8-C157-41C2-ACBA-8D1B9959FA38}">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="19.7109375" customWidth="1"/>
+    <col min="1" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -908,10 +841,10 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -919,99 +852,99 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" s="1">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" s="1">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="F5" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
@@ -1019,59 +952,59 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -1079,19 +1012,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
@@ -1099,39 +1032,37 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -1139,19 +1070,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -1159,19 +1090,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F15" s="1">
         <v>3</v>
@@ -1179,19 +1110,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -1199,19 +1130,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -1219,19 +1150,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
@@ -1239,19 +1170,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -1259,59 +1190,59 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F20" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="F21" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="F22" s="1">
         <v>5</v>
@@ -1319,19 +1250,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
@@ -1339,19 +1270,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
@@ -1359,19 +1290,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="F25" s="1">
         <v>2</v>
@@ -1379,19 +1310,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
@@ -1399,19 +1330,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
@@ -1419,19 +1350,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="F28" s="1">
         <v>1</v>
@@ -1439,19 +1370,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
@@ -1459,19 +1390,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
@@ -1479,19 +1410,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
@@ -1499,19 +1430,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Schematic Corrections and Layout Revision
Addressed significant errors discovered in the schematic. Recommended a thorough review at this juncture. Also, made corresponding adjustments to the layout accordingly.
</commit_message>
<xml_diff>
--- a/hardware/altium/Project Outputs for AirPurity/BOM/Bill of Materials-AirPurity.xlsx
+++ b/hardware/altium/Project Outputs for AirPurity/BOM/Bill of Materials-AirPurity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\GitHub\AirPurity\hardware\altium\Project Outputs for AirPurity\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1095F897-0C2C-41F6-88AE-3BEBB01EE6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{82CB31CA-63FA-4B61-909A-0B412628FAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="0" windowWidth="28800" windowHeight="15345" xr2:uid="{4B2EE2B4-5E0D-4A31-88AE-D919FA95C19D}"/>
+    <workbookView xWindow="1260" yWindow="0" windowWidth="28800" windowHeight="15345" xr2:uid="{B374EA10-9317-4E5F-AA33-2799FC90FE00}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-AirPurity" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="136">
   <si>
     <t>Comment</t>
   </si>
@@ -59,16 +59,16 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>ANT016008LCS2442MA2</t>
-  </si>
-  <si>
-    <t>RF ANT 2.4GHZ</t>
+    <t>2450AT18A100</t>
+  </si>
+  <si>
+    <t>Chip Antenna 0.5dBi 2.4GHz 2W 1206</t>
   </si>
   <si>
     <t>ANT1</t>
   </si>
   <si>
-    <t>C209892</t>
+    <t>C89334</t>
   </si>
   <si>
     <t>GRM155R61E105KA12D</t>
@@ -77,7 +77,7 @@
     <t>1uF X5R 0402 Multilayer Ceramic Capacitor</t>
   </si>
   <si>
-    <t>C1, C6, C10, C11, C12, C13, C14, C19, C20, C22, C23, C24, C25, C27, C29, C30, C32</t>
+    <t>C1, C10, C11, C12, C13, C14, C19, C20, C22, C23, C24, C25, C27, C29, C30, C32, C39</t>
   </si>
   <si>
     <t>C77009</t>
@@ -89,46 +89,58 @@
     <t>4.7uF X5R 0402 Multilayer Ceramic Capacitor</t>
   </si>
   <si>
-    <t>C2, C3, C26, C31</t>
+    <t>C2, C3, C4, C26, C31</t>
   </si>
   <si>
     <t>C2858031</t>
   </si>
   <si>
+    <t>GRM0335C1H150FA01D</t>
+  </si>
+  <si>
+    <t>15pF C0G 0201 Multilayer Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>C5, C7, C33, C34</t>
+  </si>
+  <si>
+    <t>C237567</t>
+  </si>
+  <si>
     <t>GRM033R61A104KE15D</t>
   </si>
   <si>
     <t>100nF X5R 0201 Multilayer Ceramic Capacitor</t>
   </si>
   <si>
-    <t>C4, C8, C9, C15, C16, C17, C18, C21, C28, C37</t>
+    <t>C6, C8, C9, C15, C16, C17, C18, C21, C28, C37</t>
   </si>
   <si>
     <t>C76934</t>
   </si>
   <si>
-    <t>GRM0335C1H150FA01D</t>
-  </si>
-  <si>
-    <t>15pF C0G 0201 Multilayer Ceramic Capacitor</t>
-  </si>
-  <si>
-    <t>C5, C7, C33, C34</t>
-  </si>
-  <si>
-    <t>C237567</t>
-  </si>
-  <si>
-    <t>GRM0335C1H180FA01D</t>
-  </si>
-  <si>
-    <t>18pF C0G 0201 Multilayer Ceramic Capacitor</t>
+    <t>GRM0335C1H100JA01D</t>
+  </si>
+  <si>
+    <t>10pF C0G 0201 Multilayer Ceramic Capacitor</t>
   </si>
   <si>
     <t>C35, C36</t>
   </si>
   <si>
-    <t>C384967</t>
+    <t>C76921</t>
+  </si>
+  <si>
+    <t>GRM0335C1H1R0BA01D</t>
+  </si>
+  <si>
+    <t>1pF C0G 0201 Multilayer Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>C38</t>
+  </si>
+  <si>
+    <t>C85893</t>
   </si>
   <si>
     <t>MBR0530T3G</t>
@@ -209,16 +221,28 @@
     <t>C122394</t>
   </si>
   <si>
-    <t>LQP03TN2N1BZ2D</t>
-  </si>
-  <si>
-    <t>Inductor 2.1nH</t>
-  </si>
-  <si>
-    <t>L1, L2, L3</t>
-  </si>
-  <si>
-    <t>C560038</t>
+    <t>LQP03TN3N9B02D</t>
+  </si>
+  <si>
+    <t>Inductor 3.9nH</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>C77115</t>
+  </si>
+  <si>
+    <t>LQP03TG2N7C02D</t>
+  </si>
+  <si>
+    <t>Inductor 2.7nH</t>
+  </si>
+  <si>
+    <t>L2, L3</t>
+  </si>
+  <si>
+    <t>C337946</t>
   </si>
   <si>
     <t>1239AS-H-100M=P2</t>
@@ -299,7 +323,7 @@
     <t>10kΩ 0402 Chip Resistor</t>
   </si>
   <si>
-    <t>R4, R5, R11, R12, R14</t>
+    <t>R4, R5, R11, R12, R14, R15</t>
   </si>
   <si>
     <t>C60490</t>
@@ -818,8 +842,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E378B09-E1DA-4C08-9836-1932D415E434}">
-  <dimension ref="A1:F32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A96E0CD-B576-4713-B308-F2F9BF7C0FF8}">
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -907,7 +931,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -927,7 +951,7 @@
         <v>21</v>
       </c>
       <c r="F5" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -947,7 +971,7 @@
         <v>25</v>
       </c>
       <c r="F6" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -987,7 +1011,7 @@
         <v>33</v>
       </c>
       <c r="F8" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,7 +1031,7 @@
         <v>37</v>
       </c>
       <c r="F9" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1055,37 +1079,37 @@
         <v>46</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F12" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1125,7 +1149,7 @@
         <v>59</v>
       </c>
       <c r="F15" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1165,7 +1189,7 @@
         <v>67</v>
       </c>
       <c r="F17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1225,7 +1249,7 @@
         <v>79</v>
       </c>
       <c r="F20" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1245,7 +1269,7 @@
         <v>83</v>
       </c>
       <c r="F21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1265,7 +1289,7 @@
         <v>87</v>
       </c>
       <c r="F22" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1305,7 +1329,7 @@
         <v>95</v>
       </c>
       <c r="F24" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1365,7 +1389,7 @@
         <v>107</v>
       </c>
       <c r="F27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1465,6 +1489,46 @@
         <v>127</v>
       </c>
       <c r="F32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F34" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>